<commit_message>
Code readability Feedback: 1. Add comment for each method
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58457C38-4A96-43A9-A7CB-42510BC4C7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB671642-718A-4210-BC49-30858A6D0CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Exception Handling" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -460,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD2B375-D94B-4FC8-B948-81ECE876AC4D}">
   <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,4 +612,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6FC33B-2857-4EE0-A484-922E65EB5B1F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exception Controller Feedback4: 1. Use specific exception types: Instead of catching general  Exception , try to catch more specific exceptions that can occur in your code. For example, if  taskService.getAllTasks()  can throw a specific exception like  TaskServiceException , catch that instead of a general  Exception .
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB671642-718A-4210-BC49-30858A6D0CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4348CCA8-69C0-4082-B2BD-803EB76B57EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -101,12 +101,30 @@
       <t xml:space="preserve"> Implement robust exception handling to provide meaningful error responses to clients. Use custom exception classes and exception handlers to handle various error scenarios gracefully.</t>
     </r>
   </si>
+  <si>
+    <t>Exception Controller Feedback1: …</t>
+  </si>
+  <si>
+    <t>1. Add basic exception with try catch and centerialized method</t>
+  </si>
+  <si>
+    <t>Exception Controller Feedback2: …</t>
+  </si>
+  <si>
+    <t>1. Should create different exception handling for different type of error</t>
+  </si>
+  <si>
+    <t>Exception Controller Feedback3: …</t>
+  </si>
+  <si>
+    <t>1. GlobalExceptionHandler for complex application and with mutliple controller, direct exception in controller is also fine</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +139,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7D8590"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,13 +172,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -616,14 +659,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6FC33B-2857-4EE0-A484-922E65EB5B1F}">
-  <dimension ref="A1"/>
+  <dimension ref="C3:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="57.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://github.com/pankajproject99/productionGrade/commit/231e709e02a1078c5235237db7e1fe747f969625" xr:uid="{24DD54FE-A728-4522-8CF3-5BF9CA644E6E}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://github.com/pankajproject99/productionGrade/commit/541d4c04fb19e7d0a9d35e01ad8b1bd9103e7bde" xr:uid="{D013D91A-2806-4633-8603-E4A09CD67045}"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://github.com/pankajproject99/productionGrade/commit/0340707bd1418d600dab2f3c44696f0f9e66ad21" xr:uid="{150343D4-D276-4985-AA4A-714E7064947E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Validate Feedback 1 @Valid : 1. Use @Valid build in validation and for Exception MethodArgumentNotValidException
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4348CCA8-69C0-4082-B2BD-803EB76B57EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB770E4-3352-487C-8107-FF6E8FCA0AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Exception Handling" sheetId="2" r:id="rId2"/>
+    <sheet name="Design" sheetId="4" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="1. Exception Handling" sheetId="2" r:id="rId3"/>
+    <sheet name="2.Validation" sheetId="5" r:id="rId4"/>
+    <sheet name="VehicleCarCycle" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -119,12 +122,469 @@
   <si>
     <t>1. GlobalExceptionHandler for complex application and with mutliple controller, direct exception in controller is also fine</t>
   </si>
+  <si>
+    <t>After Fixing Above there are still below suggestions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Use specific exception types: Instead of catching general  Exception , try to catch more specific exceptions that can occur in your code. For example, if  taskService.getAllTasks()  can throw a specific exception like  TaskServiceException , catch that instead of a general  Exception . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Provide more detailed error messages: Consider providing more detailed error messages in your exception handling methods. This can help in troubleshooting and debugging when issues occur. Include relevant information such as the specific request or operation that caused the exception. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Use appropriate HTTP status codes: While your code already uses appropriate HTTP status codes for different exception types, you can further enhance it by using more specific status codes. For example, if a task is not found, you can use  HttpStatus.NOT_FOUND  instead of  HttpStatus.INTERNAL_SERVER_ERROR  in the  markTaskAsCompleted  method. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Consider using custom exception classes: Instead of using generic exception classes like  RuntimeException ,  BadRequestException , and  NotFoundException , you can create custom exception classes that provide more context-specific information. This can make your code more readable and maintainable. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Add logging: It's a good practice to log exceptions and error messages for debugging and monitoring purposes. Consider adding logging statements to log the exception stack trace or error messages when an exception occurs. </t>
+  </si>
+  <si>
+    <t>6. Use Enumerations for Error Codes: Instead of relying solely on string-based error messages, consider using an enumeration or constants for defining error codes. This provides a more standardized and maintainable way to handle and identify different types of errors.</t>
+  </si>
+  <si>
+    <t>7. Distinguish Between Business and Technical Errors: Consider categorizing exceptions into two main types: business errors and technical errors. Business errors represent issues related to the application's logic (e.g., invalid input), while technical errors represent issues with the application's infrastructure (e.g., database connection failure). Handling and presenting these errors differently can help users and developers understand and address them more effectively.</t>
+  </si>
+  <si>
+    <t>8. make error reponse generic by creating as object</t>
+  </si>
+  <si>
+    <t>Bard</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>VehicleType</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>VehicleService</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>VehicleController</t>
+  </si>
+  <si>
+    <t>CAR, CYCLE</t>
+  </si>
+  <si>
+    <t>if(vehicleType car) = return new Car(model)</t>
+  </si>
+  <si>
+    <t>if(vehicleType cycle) = return new Cycle(model)</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Dto</t>
+  </si>
+  <si>
+    <t>VehicleInputDto</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>ModelMapper</t>
+  </si>
+  <si>
+    <t>Vehicle and VehicleDto</t>
+  </si>
+  <si>
+    <t>VehicleOutputDto</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>VehicleBatchJob</t>
+  </si>
+  <si>
+    <t>Class Car</t>
+  </si>
+  <si>
+    <t>extends Vehicle</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>super("CAR", model)</t>
+  </si>
+  <si>
+    <t>ModelMapperService</t>
+  </si>
+  <si>
+    <r>
+      <t>public</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">class ModelMapperService </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>private</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>final</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ModelMapper modelMapper; public ModelMapperService() { </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>this</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.modelMapper = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ModelMapper(); modelMapper.addMappings(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> AbstractMap&lt;String, PropertyMap&gt;() { </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Override</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> protected void populate() { map(Vehicle.class).typeMap(VehicleOutputDto.class) .addMapping(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"type"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"type"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, String.class); } }); } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>public</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;T&gt; T map(Object source, Class&lt;T&gt; targetClass) { </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFC4C7C5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> modelMapper.map(source, targetClass); } }</t>
+    </r>
+  </si>
+  <si>
+    <t>Class Cycle</t>
+  </si>
+  <si>
+    <t>super("CYCLE", model)</t>
+  </si>
+  <si>
+    <t>Dao Interface</t>
+  </si>
+  <si>
+    <t>VehicleDao</t>
+  </si>
+  <si>
+    <t>Dao Impl</t>
+  </si>
+  <si>
+    <t>VehicleDaoImpl</t>
+  </si>
+  <si>
+    <t>Table: vehicles Columns: id: Long (primary key) type: String model: String</t>
+  </si>
+  <si>
+    <t>Dao Dto</t>
+  </si>
+  <si>
+    <t>VehicleDto</t>
+  </si>
+  <si>
+    <t>Exception Controller Feedback5: </t>
+  </si>
+  <si>
+    <t>Exception Controller Feedback4:</t>
+  </si>
+  <si>
+    <t>Exception Controller Feedback6: </t>
+  </si>
+  <si>
+    <t>1. Use specific exception types: Instead of catching general  Exception , try to catch more specific exceptions that can occur in your code. For example, if  taskService.getAllTasks()  can throw a specific exception like  TaskServiceException , catch that instead of a general  Exception .</t>
+  </si>
+  <si>
+    <t>The code could be more modular. The code is currently written as a single large file. It would be better to break the code up into smaller, more reusable modules. This would make the code easier to maintain and update.</t>
+  </si>
+  <si>
+    <t>The code could be more documented. The code currently has very little documentation. It would be helpful to add comments to the code to explain what it is doing and why. This would make the code easier for other developers to understand and maintain.</t>
+  </si>
+  <si>
+    <t>The code could be tested more thoroughly. The code currently has a few unit tests, but it would be good to add more tests to cover all of the possible cases. This would help to ensure that the code is working as expected.</t>
+  </si>
+  <si>
+    <t>TaskController</t>
+  </si>
+  <si>
+    <t>TaskService</t>
+  </si>
+  <si>
+    <t>CreateTaskRequest</t>
+  </si>
+  <si>
+    <t>TaskMapper</t>
+  </si>
+  <si>
+    <t>TaskResponse</t>
+  </si>
+  <si>
+    <t>Endpoint Input</t>
+  </si>
+  <si>
+    <t>DaoInput</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>ControllerInput</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>CreateTaskRequest, Task</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>DaoOutput</t>
+  </si>
+  <si>
+    <t>ControllerOutput</t>
+  </si>
+  <si>
+    <t>Task, TaskResponse</t>
+  </si>
+  <si>
+    <t>Dao</t>
+  </si>
+  <si>
+    <t>TaskRepository</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Validation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Validate input data, both in the controller and service layers. Use annotations like @Valid and validation frameworks to ensure that the input meets the expected criteria.</t>
+    </r>
+  </si>
+  <si>
+    <t>Use @Valid build in validation and for Exception MethodArgumentNotValidException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Feedback 1 @Valid : </t>
+  </si>
+  <si>
+    <t>1. Use @Valid build in validation and for Exception MethodArgumentNotValidException</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +614,24 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFC4C7C5"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -186,6 +664,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -501,21 +985,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD2B375-D94B-4FC8-B948-81ECE876AC4D}">
-  <dimension ref="B2:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156CAB31-392D-444C-BC88-7028FFD19127}">
+  <dimension ref="C4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:6">
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6">
+      <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6">
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD2B375-D94B-4FC8-B948-81ECE876AC4D}">
+  <dimension ref="B2:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -523,15 +1131,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -539,7 +1147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -547,7 +1155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -555,7 +1163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -563,7 +1171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -571,7 +1179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -579,7 +1187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -587,7 +1195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12">
         <v>10</v>
       </c>
@@ -595,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3">
       <c r="B13">
         <v>11</v>
       </c>
@@ -603,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -611,7 +1219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3">
       <c r="B15">
         <v>13</v>
       </c>
@@ -619,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3">
       <c r="B16">
         <v>14</v>
       </c>
@@ -627,7 +1235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17">
         <v>15</v>
       </c>
@@ -635,7 +1243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3">
       <c r="B18">
         <v>16</v>
       </c>
@@ -643,12 +1251,41 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -657,20 +1294,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6FC33B-2857-4EE0-A484-922E65EB5B1F}">
-  <dimension ref="C3:D6"/>
+  <dimension ref="C3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:4">
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
@@ -678,7 +1315,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:4">
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
@@ -686,7 +1323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4">
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
@@ -694,15 +1331,345 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="3"/>
+    <row r="6" spans="3:4">
+      <c r="C6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="3:4">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4">
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4">
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4">
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4">
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4">
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="https://github.com/pankajproject99/productionGrade/commit/231e709e02a1078c5235237db7e1fe747f969625" xr:uid="{24DD54FE-A728-4522-8CF3-5BF9CA644E6E}"/>
     <hyperlink ref="C4" r:id="rId2" display="https://github.com/pankajproject99/productionGrade/commit/541d4c04fb19e7d0a9d35e01ad8b1bd9103e7bde" xr:uid="{D013D91A-2806-4633-8603-E4A09CD67045}"/>
     <hyperlink ref="C5" r:id="rId3" display="https://github.com/pankajproject99/productionGrade/commit/0340707bd1418d600dab2f3c44696f0f9e66ad21" xr:uid="{150343D4-D276-4985-AA4A-714E7064947E}"/>
+    <hyperlink ref="C20" r:id="rId4" display="https://github.com/pankajproject99/productionGrade/commit/a4a94480d7f71941d014dc48342602d9f65e70a6" xr:uid="{075B2CDD-0740-42DB-9B17-E2A24F179BC2}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://github.com/pankajproject99/productionGrade/commit/ad0a80d7d8cf36269cacb00abacc826cb6317de2" xr:uid="{1FC9276F-7489-4DBB-B008-65D4D1F10A3D}"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://github.com/pankajproject99/productionGrade/commit/a4a94480d7f71941d014dc48342602d9f65e70a6" xr:uid="{75225801-4BB2-4340-ABB0-489701167740}"/>
+    <hyperlink ref="C8" r:id="rId7" display="https://github.com/pankajproject99/productionGrade/commit/e63e46e4517abe348669c810c05c2afe1a98baef" xr:uid="{DD1E529D-CC1B-4D17-9566-85569D62DF26}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0501FF-D880-4C9B-911E-55AE0DEB151B}">
+  <dimension ref="B2:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="25.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC957D7F-2009-4CCE-B0DC-85483296FB4B}">
+  <dimension ref="B2:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="D12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Validate Feedback 2 @Validate : Use @Validate and provide custom message and POST check input should not be null and call custom application validation Solution: HandlerInterceptor.prehandle
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB770E4-3352-487C-8107-FF6E8FCA0AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E19D3A-E4EC-4331-A40C-070F0E1C2886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -578,6 +578,18 @@
   </si>
   <si>
     <t>1. Use @Valid build in validation and for Exception MethodArgumentNotValidException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Feedback 2 @Validate : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Use @Validate and provide custom message </t>
+  </si>
+  <si>
+    <t>Use @Validate and provide custom message and POST check input should not be null and call custom application validation</t>
+  </si>
+  <si>
+    <t>Solution: HandlerInterceptor.prehandle</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1001,7 @@
   <dimension ref="C4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1443,15 +1455,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0501FF-D880-4C9B-911E-55AE0DEB151B}">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -1470,12 +1482,38 @@
         <v>99</v>
       </c>
     </row>
+    <row r="5" spans="2:5">
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="18" spans="3:4">
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validate Feedback 3 Business Validation : 3. Create a separate class with application business level validation
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E19D3A-E4EC-4331-A40C-070F0E1C2886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDF3F2B-AC9C-4872-979D-6B61C5C9889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -590,6 +590,42 @@
   </si>
   <si>
     <t>Solution: HandlerInterceptor.prehandle</t>
+  </si>
+  <si>
+    <t>validate</t>
+  </si>
+  <si>
+    <t>HandlerInterceptor preHandle</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>ValidationInterceptor</t>
+  </si>
+  <si>
+    <t>TaskRequestValidator</t>
+  </si>
+  <si>
+    <t>Business level valiadation which can be placed in controller or service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Feedback 3 Business Validation : </t>
+  </si>
+  <si>
+    <t>Create a separate class with application business level validation</t>
+  </si>
+  <si>
+    <t>3. Create a separate class with application business level validation</t>
+  </si>
+  <si>
+    <t>config</t>
+  </si>
+  <si>
+    <t>AppConfig</t>
+  </si>
+  <si>
+    <t>register interceptor</t>
   </si>
 </sst>
 </file>
@@ -998,16 +1034,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156CAB31-392D-444C-BC88-7028FFD19127}">
-  <dimension ref="C4:F14"/>
+  <dimension ref="C4:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.6328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1115,8 +1151,42 @@
         <v>86</v>
       </c>
     </row>
+    <row r="16" spans="3:6">
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1125,7 +1195,7 @@
   <dimension ref="B2:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1457,13 +1527,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0501FF-D880-4C9B-911E-55AE0DEB151B}">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="29.6328125" customWidth="1"/>
+    <col min="4" max="4" width="37.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -1490,6 +1560,14 @@
         <v>101</v>
       </c>
     </row>
+    <row r="6" spans="2:5">
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="18" spans="3:4">
       <c r="C18">
         <v>1</v>
@@ -1514,6 +1592,9 @@
     <row r="21" spans="3:4">
       <c r="C21">
         <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Security Feedback 1: 1. Authentication(who) and Authorization(prevs or what is allowed) with JWT Token, should allow permit all for token url and rest should Authenticate
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDF3F2B-AC9C-4872-979D-6B61C5C9889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B027C630-B3A0-44CA-9BAC-C73484D8C1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="4" r:id="rId1"/>
     <sheet name="Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="1. Exception Handling" sheetId="2" r:id="rId3"/>
-    <sheet name="2.Validation" sheetId="5" r:id="rId4"/>
-    <sheet name="VehicleCarCycle" sheetId="3" r:id="rId5"/>
+    <sheet name="17. Code Review" sheetId="6" r:id="rId3"/>
+    <sheet name="1. Exception Handling" sheetId="2" r:id="rId4"/>
+    <sheet name="2.Validation" sheetId="5" r:id="rId5"/>
+    <sheet name="3. Security" sheetId="7" r:id="rId6"/>
+    <sheet name="VehicleCarCycle" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="162">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -610,9 +612,6 @@
     <t>Business level valiadation which can be placed in controller or service</t>
   </si>
   <si>
-    <t xml:space="preserve">Validate Feedback 3 Business Validation : </t>
-  </si>
-  <si>
     <t>Create a separate class with application business level validation</t>
   </si>
   <si>
@@ -626,13 +625,154 @@
   </si>
   <si>
     <t>register interceptor</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>develop</t>
+  </si>
+  <si>
+    <t>PR @ChatGpt</t>
+  </si>
+  <si>
+    <t>Code Style</t>
+  </si>
+  <si>
+    <t>Declaration Redundancy</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Java Language Level migration aids</t>
+  </si>
+  <si>
+    <t>Probable Bugs</t>
+  </si>
+  <si>
+    <t>Field may be final</t>
+  </si>
+  <si>
+    <t>Declaration Can be final</t>
+  </si>
+  <si>
+    <t>Empty Methods</t>
+  </si>
+  <si>
+    <t>Ununes Declaration</t>
+  </si>
+  <si>
+    <t>Unused Imports</t>
+  </si>
+  <si>
+    <t>Class can be records</t>
+  </si>
+  <si>
+    <t>Pattern Variable can be used</t>
+  </si>
+  <si>
+    <t>Function may return null</t>
+  </si>
+  <si>
+    <t>Validate Feedback 3 Business Validation :</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>UserRepository</t>
+  </si>
+  <si>
+    <t>https://medium.com/@truongbui95/jwt-authentication-and-authorization-with-spring-boot-3-and-spring-security-6-2f90f9337421</t>
+  </si>
+  <si>
+    <t>Entities</t>
+  </si>
+  <si>
+    <t>Repo</t>
+  </si>
+  <si>
+    <t>request: SigininRequest</t>
+  </si>
+  <si>
+    <t>request: SiginUpRequest</t>
+  </si>
+  <si>
+    <t>response:JwtAuthenticationResponse</t>
+  </si>
+  <si>
+    <t>AuthenticationController</t>
+  </si>
+  <si>
+    <t>signup, signin</t>
+  </si>
+  <si>
+    <t>AuthenticationService</t>
+  </si>
+  <si>
+    <t>JwtService</t>
+  </si>
+  <si>
+    <t>UserService</t>
+  </si>
+  <si>
+    <t>using UserRepository, using JwtService, using PasswordEncoder, using AuthenticationManager</t>
+  </si>
+  <si>
+    <t>JwtAuthencationFilter</t>
+  </si>
+  <si>
+    <t>SecurityConfiguration</t>
+  </si>
+  <si>
+    <t>using JwtService, using UserService</t>
+  </si>
+  <si>
+    <t>using JwtAuthenticationFilter, using UserService</t>
+  </si>
+  <si>
+    <t>intercepts request and is custom SecurityFilterChain</t>
+  </si>
+  <si>
+    <t>to match api/url</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>@RequiredArgsConstructor</t>
+  </si>
+  <si>
+    <t>'@Builder</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>Spring Security with JWT token</t>
+  </si>
+  <si>
+    <t>Security Feedback 1:</t>
+  </si>
+  <si>
+    <t>1. Authentication(who) and Authorization(prevs or what is allowed) with JWT Token, should allow permit all for token url and rest should Authenticate1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,6 +820,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF643820"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -702,7 +848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -719,6 +865,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1034,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156CAB31-392D-444C-BC88-7028FFD19127}">
-  <dimension ref="C4:F18"/>
+  <dimension ref="C4:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1175,13 +1324,37 @@
     </row>
     <row r="18" spans="3:5">
       <c r="C18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" t="s">
         <v>113</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>114</v>
       </c>
-      <c r="E18" t="s">
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
+      <c r="C21" t="s">
         <v>115</v>
+      </c>
+      <c r="D21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="D22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1368,7 @@
   <dimension ref="B2:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1377,6 +1550,126 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43E4DDC-A55D-4D47-AAE6-3F07A7AAB1A0}">
+  <dimension ref="C3:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6">
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6FC33B-2857-4EE0-A484-922E65EB5B1F}">
   <dimension ref="C3:D24"/>
   <sheetViews>
@@ -1523,12 +1816,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0501FF-D880-4C9B-911E-55AE0DEB151B}">
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1561,11 +1854,11 @@
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="D6" t="s">
-        <v>110</v>
+      <c r="D6" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="3:4">
@@ -1594,15 +1887,174 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" display="https://github.com/pankajproject99/productionGrade/commit/19b26f9be458f3836ce561ac50100483647711ee" xr:uid="{FC32372B-44E5-42E1-9FD1-EFA503CD0B5E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49B197D-1E90-4D9E-A663-596B1FC97E92}">
+  <dimension ref="B2:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="43.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="C8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="C15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="C22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="C23" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="C24" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC957D7F-2009-4CCE-B0DC-85483296FB4B}">
   <dimension ref="B2:M17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Security Feedback 3: fix h2_console
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B027C630-B3A0-44CA-9BAC-C73484D8C1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAB4D31-58B4-416A-895B-A650512BDCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="166">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -766,6 +766,38 @@
   </si>
   <si>
     <t>1. Authentication(who) and Authorization(prevs or what is allowed) with JWT Token, should allow permit all for token url and rest should Authenticate1</t>
+  </si>
+  <si>
+    <t>Security Feedback 2:</t>
+  </si>
+  <si>
+    <t>2. @Valid for user signup and comment for EXPIRATRION(Bard feedback)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Security:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Implement authentication and authorization mechanisms to secure your API. Use Spring Security to control access to endpoints, and consider using tokens, OAuth, or other authentication methods.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Add role to table and during signup, verify some endpoint to be only available to ADMIN, prevent same user signup, permit h2-console </t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1431,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -1900,10 +1932,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49B197D-1E90-4D9E-A663-596B1FC97E92}">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1932,119 +1964,132 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="C8" t="s">
-        <v>135</v>
+    <row r="5" spans="2:4">
+      <c r="C5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="D6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
         <v>139</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
-      <c r="B10" t="s">
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
-      <c r="C11" t="s">
+    <row r="13" spans="2:4">
+      <c r="C13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
-      <c r="C12" t="s">
+    <row r="14" spans="2:4">
+      <c r="C14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
-      <c r="B13" t="s">
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>143</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
-      <c r="B14" t="s">
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>145</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
-      <c r="C15" t="s">
+    <row r="17" spans="2:5">
+      <c r="C17" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="C16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="C18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="C20" t="s">
         <v>150</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>152</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" t="s">
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="C22" t="s">
+    <row r="24" spans="2:5">
+      <c r="C24" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
-      <c r="C23" s="9" t="s">
+    <row r="25" spans="2:5">
+      <c r="C25" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
-      <c r="C24" s="10" t="s">
+    <row r="26" spans="2:5">
+      <c r="C26" s="10" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Security Feedback 3: 3. Add role to table and during signup, verify some endpoint to be only available to ADMIN, prevent same user signup, permit h2-console
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAB4D31-58B4-416A-895B-A650512BDCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC993E-2662-4040-823E-419B4CA8B72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="167">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -798,6 +798,9 @@
   </si>
   <si>
     <t xml:space="preserve">3. Add role to table and during signup, verify some endpoint to be only available to ADMIN, prevent same user signup, permit h2-console </t>
+  </si>
+  <si>
+    <t>Security Feedback 3:</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1938,7 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1973,6 +1976,9 @@
       </c>
     </row>
     <row r="6" spans="2:4">
+      <c r="C6" t="s">
+        <v>166</v>
+      </c>
       <c r="D6" t="s">
         <v>165</v>
       </c>

</xml_diff>

<commit_message>
Security Feedback 3a: Add validation for email to be not empty
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC993E-2662-4040-823E-419B4CA8B72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E196E2B7-2E8E-4C9A-B87A-AA871FF88B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="169">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -801,6 +801,12 @@
   </si>
   <si>
     <t>Security Feedback 3:</t>
+  </si>
+  <si>
+    <t>Security Feedback 3a:</t>
+  </si>
+  <si>
+    <t>Add validation for email to be not empty</t>
   </si>
 </sst>
 </file>
@@ -1935,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49B197D-1E90-4D9E-A663-596B1FC97E92}">
-  <dimension ref="B2:E26"/>
+  <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1983,119 +1989,127 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
-      <c r="B9" t="s">
+    <row r="7" spans="2:4">
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
         <v>138</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
-      <c r="C10" t="s">
+    <row r="11" spans="2:4">
+      <c r="C11" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="C13" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="C15" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>145</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="C18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="C19" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
         <v>112</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>149</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="C20" t="s">
+    <row r="21" spans="2:5">
+      <c r="C21" t="s">
         <v>150</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" t="s">
+    <row r="23" spans="2:5">
+      <c r="B23" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
-      <c r="C24" t="s">
+    <row r="25" spans="2:5">
+      <c r="C25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
-      <c r="C25" s="9" t="s">
+    <row r="26" spans="2:5">
+      <c r="C26" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
-      <c r="C26" s="10" t="s">
+    <row r="27" spans="2:5">
+      <c r="C27" s="10" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Validate Feedback 4 postHandle :  4. Add postHandle logging
</commit_message>
<xml_diff>
--- a/ProductionGradeSpringBootApi.xlsx
+++ b/ProductionGradeSpringBootApi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project_workspace\tutorials\chatgpt\productionGrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E196E2B7-2E8E-4C9A-B87A-AA871FF88B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5838B5EE-7651-496C-9402-0F650055EB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="4" xr2:uid="{801B3EEB-C364-4A1B-80D6-D1FF7A141F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="1. Exception Handling" sheetId="2" r:id="rId4"/>
     <sheet name="2.Validation" sheetId="5" r:id="rId5"/>
     <sheet name="3. Security" sheetId="7" r:id="rId6"/>
-    <sheet name="VehicleCarCycle" sheetId="3" r:id="rId7"/>
+    <sheet name="4. Logging" sheetId="8" r:id="rId7"/>
+    <sheet name="VehicleCarCycle" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="172">
   <si>
     <t>Production Grade Application</t>
   </si>
@@ -807,6 +808,15 @@
   </si>
   <si>
     <t>Add validation for email to be not empty</t>
+  </si>
+  <si>
+    <t>Logging:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Feedback 4 postHandle : </t>
+  </si>
+  <si>
+    <t>4. Add postHandle logging</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1419,7 @@
   <dimension ref="B2:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1861,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0501FF-D880-4C9B-911E-55AE0DEB151B}">
   <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1900,6 +1910,14 @@
       </c>
       <c r="E6" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="D7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="3:4">
@@ -1943,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49B197D-1E90-4D9E-A663-596B1FC97E92}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2120,6 +2138,37 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9B3892-36E3-4230-83A0-A2DB57F30B21}">
+  <dimension ref="B2:F9"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC957D7F-2009-4CCE-B0DC-85483296FB4B}">
   <dimension ref="B2:M17"/>
   <sheetViews>

</xml_diff>